<commit_message>
analysis in JASP done right
</commit_message>
<xml_diff>
--- a/manuscript/tableformatting.xlsx
+++ b/manuscript/tableformatting.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine Nussbaum\Documents\Arbeit\Forschungsprojekte\2025_Musicality_Singers\manuscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Christine\Arbeit\06_Forschungsprojekte\2025_Musicality_SingInstr\manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE7B0A-5A42-403B-B872-1B3BEA8271C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6200F66D-7946-434D-A8FF-32138882964E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31290" yWindow="2145" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVA" sheetId="3" r:id="rId1"/>
+    <sheet name="Correlations" sheetId="4" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>Group</t>
   </si>
@@ -208,11 +221,101 @@
   <si>
     <t>.20 [.14 .25]</t>
   </si>
+  <si>
+    <t>Cor</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>p_corrected2</t>
+  </si>
+  <si>
+    <t>F0</t>
+  </si>
+  <si>
+    <t>PROMS_Averaged</t>
+  </si>
+  <si>
+    <t>Averaged</t>
+  </si>
+  <si>
+    <t>Rhythm</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Melody</t>
+  </si>
+  <si>
+    <t>Timbre</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>0.39 (0.003)</t>
+  </si>
+  <si>
+    <t>0.38 (0.003)</t>
+  </si>
+  <si>
+    <t>0.36 (0.003)</t>
+  </si>
+  <si>
+    <t>0.35 (0.005)</t>
+  </si>
+  <si>
+    <t>0.34 (0.006)</t>
+  </si>
+  <si>
+    <t>0.32 (0.008)</t>
+  </si>
+  <si>
+    <t>0.28 (0.023)</t>
+  </si>
+  <si>
+    <t>0.27 (0.023)</t>
+  </si>
+  <si>
+    <t>0.24 (0.053)</t>
+  </si>
+  <si>
+    <t>0.23 (0.058)</t>
+  </si>
+  <si>
+    <t>0.22 (0.062)</t>
+  </si>
+  <si>
+    <t>0.22 (0.066)</t>
+  </si>
+  <si>
+    <t>0.18 (0.124)</t>
+  </si>
+  <si>
+    <t>0.15 (0.204)</t>
+  </si>
+  <si>
+    <t>0.14 (0.212)</t>
+  </si>
+  <si>
+    <t>0.08 (0.499)</t>
+  </si>
+  <si>
+    <t>0.08 (0.503)</t>
+  </si>
+  <si>
+    <t>0.05 (0.673)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -294,21 +397,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -591,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94C82FD-D3EE-4A7D-8BD7-8F31A56C3156}">
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -606,10 +705,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="6"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -642,7 +741,7 @@
       <c r="D3" s="1">
         <v>86</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="3">
         <v>0.375</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -651,7 +750,7 @@
       <c r="G3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -663,7 +762,7 @@
       <c r="D4" s="1">
         <v>258</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="3">
         <v>72.430000000000007</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -714,7 +813,7 @@
       <c r="G6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1018,4 +1117,511 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD06323-5469-48A0-BB42-6D72B416199E}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.39497611999999999</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2.6397769999999998E-3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.38173840999999997</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2.6397769999999998E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.36499183000000002</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3.3941710000000001E-3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.34804257</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4.7778630000000002E-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.33692074</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5.6717019999999998E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.32032853</v>
+      </c>
+      <c r="D7" s="9">
+        <v>7.9689089999999997E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.31684917000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7.9689089999999997E-3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.27783933</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2.2932061E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.27341378</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2.3102238000000001E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.23767758999999999</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5.3285411999999997E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.22993889000000001</v>
+      </c>
+      <c r="D12" s="9">
+        <v>5.8459993000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.22357933999999999</v>
+      </c>
+      <c r="D13" s="9">
+        <v>6.2286729999999998E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.21785922999999999</v>
+      </c>
+      <c r="D14" s="9">
+        <v>6.5621494000000002E-2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.18486996</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.123554408</v>
+      </c>
+      <c r="J15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.15365833000000001</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.203888131</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.15085072999999999</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.203888131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.14490594000000001</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.21238881100000001</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="10">
+        <v>8.2127800000000001E-2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.49945290399999998</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" t="s">
+        <v>63</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="10">
+        <v>7.7049560000000003E-2</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.50328306</v>
+      </c>
+      <c r="J20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="10">
+        <v>4.5846709999999999E-2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.67326856599999996</v>
+      </c>
+      <c r="J21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BAE2CC-0FEF-45A4-BB05-27F36BCFE45A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>